<commit_message>
Update ETL pipeline: added snapshot logic and panel data import with header handling
</commit_message>
<xml_diff>
--- a/data/Firms.xlsx
+++ b/data/Firms.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\OneDrive - National Economics University\Firm_Data_Project_group3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5688"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Trang tính1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
-  <si>
-    <t>Ticker</t>
-  </si>
-  <si>
-    <t>Firms</t>
-  </si>
-  <si>
-    <t>Exchange</t>
-  </si>
-  <si>
-    <t>Industry</t>
-  </si>
-  <si>
-    <t>Established_year</t>
-  </si>
   <si>
     <t>VGS</t>
   </si>
@@ -173,12 +158,27 @@
   <si>
     <t>CTCP Giao nhận Vận tải Ngoại thương</t>
   </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>exchange_id</t>
+  </si>
+  <si>
+    <t>ticker</t>
+  </si>
+  <si>
+    <t>established_year</t>
+  </si>
+  <si>
+    <t>industry_l2_id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -217,6 +217,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -250,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -269,6 +276,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -307,22 +315,6 @@
       </fill>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFA4FFA4"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFA4FFA4"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFA4FFA4"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFA4FFA4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFAFFD95"/>
@@ -346,13 +338,29 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFA4FFA4"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFA4FFA4"/>
+        </right>
+        <top style="thin">
+          <color rgb="FFA4FFA4"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FFA4FFA4"/>
+        </bottom>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="3">
     <tableStyle name="Trang tính1-style" pivot="0" count="4">
-      <tableStyleElement type="wholeTable" size="0" dxfId="4"/>
-      <tableStyleElement type="headerRow" dxfId="7"/>
-      <tableStyleElement type="firstRowStripe" dxfId="6"/>
-      <tableStyleElement type="secondRowStripe" dxfId="5"/>
+      <tableStyleElement type="wholeTable" size="0" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="6"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="secondRowStripe" dxfId="4"/>
     </tableStyle>
     <tableStyle name="Trang tính1-style 2" pivot="0" count="2">
       <tableStyleElement type="firstRowStripe" dxfId="3"/>
@@ -381,11 +389,11 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Firms" displayName="Firms" ref="A1:E22">
   <tableColumns count="5">
-    <tableColumn id="1" name="Ticker"/>
-    <tableColumn id="2" name="Firms"/>
-    <tableColumn id="3" name="Exchange"/>
-    <tableColumn id="4" name="Industry"/>
-    <tableColumn id="5" name="Established_year"/>
+    <tableColumn id="1" name="ticker"/>
+    <tableColumn id="2" name="company_name"/>
+    <tableColumn id="3" name="exchange_id"/>
+    <tableColumn id="4" name="industry_l2_id"/>
+    <tableColumn id="5" name="established_year"/>
   </tableColumns>
   <tableStyleInfo name="Trang tính1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -622,7 +630,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -636,19 +644,19 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -674,16 +682,16 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E2" s="4">
         <v>2002</v>
@@ -712,16 +720,16 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E3" s="4">
         <v>1999</v>
@@ -750,16 +758,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E4" s="4">
         <v>1998</v>
@@ -788,16 +796,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E5" s="4">
         <v>1967</v>
@@ -826,16 +834,16 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4">
         <v>2010</v>
@@ -864,23 +872,23 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E7" s="4">
         <v>1966</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="10"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -902,16 +910,16 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E8" s="4">
         <v>1960</v>
@@ -940,16 +948,16 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E9" s="4">
         <v>1978</v>
@@ -978,16 +986,16 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E10" s="4">
         <v>2003</v>
@@ -1016,16 +1024,16 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E11" s="4">
         <v>1978</v>
@@ -1054,16 +1062,16 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E12" s="4">
         <v>2004</v>
@@ -1092,16 +1100,16 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E13" s="4">
         <v>2003</v>
@@ -1130,16 +1138,16 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E14" s="4">
         <v>1976</v>
@@ -1168,16 +1176,16 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E15" s="4">
         <v>2001</v>
@@ -1206,16 +1214,16 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E16" s="4">
         <v>2007</v>
@@ -1244,16 +1252,16 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E17" s="4">
         <v>2006</v>
@@ -1282,16 +1290,16 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E18" s="4">
         <v>2007</v>
@@ -1320,16 +1328,16 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E19" s="4">
         <v>1975</v>
@@ -1358,16 +1366,16 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E20" s="4">
         <v>2007</v>
@@ -1396,16 +1404,16 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E21" s="4">
         <v>1996</v>

</xml_diff>